<commit_message>
added more univrsities percentage
</commit_message>
<xml_diff>
--- a/نسبـالجامعاتــالسعودية.xlsx
+++ b/نسبـالجامعاتــالسعودية.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mac/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mac/Documents/GitHub/University_percentage_admission/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="14400"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="45">
   <si>
     <t> جامعة أم القرى</t>
   </si>
@@ -114,6 +114,51 @@
   </si>
   <si>
     <t>Done</t>
+  </si>
+  <si>
+    <t>لا</t>
+  </si>
+  <si>
+    <t>https://portal.uhb.edu.sa/admitportal/PLL/admission/Pages/Page.aspx?id=14</t>
+  </si>
+  <si>
+    <t>https://ub.edu.sa/</t>
+  </si>
+  <si>
+    <t>https://registration.ub.edu.sa/bisha/files/admissionPolicies.pdf;jsessionid=MUwPgfMzRRsuwkfA4yzUvmd-TuHMZpqZRGnC1YQlWvAZmRzR_5dn!294645458</t>
+  </si>
+  <si>
+    <t>https://www.uhb.edu.sa/ar/Pages/default.aspx</t>
+  </si>
+  <si>
+    <t>https://www.uj.edu.sa/Pages-Acceptance.aspx#:~:text=%D9%85%D8%B9%D8%A7%D9%8A%D9%8A%D9%80%D8%B1%20%D8%A7%D9%84%D9%82%D8%A8%D9%80%D9%88%D9%84%20%D8%A8%D8%AC%D8%A7%D9%85%D8%B9%D8%A9%20%D8%AC%D8%AF%D8%A9%20%3A&amp;text=%D8%A7%D9%84%D8%AF%D8%B1%D8%AC%D8%A9%20%D8%A7%D9%84%D9%85%D9%88%D8%B2%D9%88%D9%86%D8%A9%20%D9%84%D9%84%D8%B3%D9%86%D8%A9%20%D8%A7%D9%84%D8%AA%D8%AD%D8%B6%D9%8A%D8%B1%D9%8A%D8%A9%20%D8%A7%D9%84%D9%85%D8%B3%D8%A7%D8%B1,%D8%AF%D8%B1%D8%AC%D8%A9%20%D8%A7%D9%84%D8%AA%D8%AD%D8%B5%D9%8A%D9%84%D9%8A%20%C3%97%2020%25).&amp;text=%D8%A7%D9%84%D8%AF%D8%B1%D8%AC%D8%A9%20%D8%A7%D9%84%D9%85%D9%88%D8%B2%D9%88%D9%86%D8%A9%20%D9%84%D9%84%D8%B3%D9%86%D8%A9%20%D8%A7%D9%84%D8%AA%D8%AD%D8%B6%D9%8A%D8%B1%D9%8A%D8%A9%20%D8%A7%D9%84%D9%85%D8%B3%D8%A7%D8%B1%20%D8%A7%D9%84%D8%A3%D8%AF%D8%A8%D9%8A%20(%D8%B7%D9%84%D8%A7%D8%A8)%20%3D%20(%20%D9%86%D8%B3%D8%A8%D8%A9,%D8%AF%D8%B1%D8%AC%D8%A9%20%D8%A7%D9%84%D9%82%D8%AF%D8%B1%D8%A7%D8%AA%20%C3%97%2040%25%20).</t>
+  </si>
+  <si>
+    <t>https://uj.edu.sa/</t>
+  </si>
+  <si>
+    <t>https://www.seu.edu.sa/ar/faqs/</t>
+  </si>
+  <si>
+    <t>https://www.seu.edu.sa/ar//</t>
+  </si>
+  <si>
+    <t>http://m.mu.edu.sa/ar/%D8%A7%D9%84%D8%A7%D8%AF%D8%A7%D8%B1%D8%A7%D8%AA/%D8%B9%D9%85%D8%A7%D8%AF%D8%A9-%D8%A7%D9%84%D9%82%D8%A8%D9%88%D9%84-%D9%88%D8%A7%D9%84%D8%AA%D8%B3%D8%AC%D9%8A%D9%84/%D9%85%D8%B9%D8%A7%D9%8A%D9%8A%D8%B1-%D8%A7%D9%84%D9%82%D8%A8%D9%88%D9%84-%D8%A8%D8%AC%D8%A7%D9%85%D8%B9%D8%A9-%D8%A7%D9%84%D9%85%D8%AC%D9%85%D8%B9%D8%A9</t>
+  </si>
+  <si>
+    <t>https://m.mu.edu.sa/ar</t>
+  </si>
+  <si>
+    <t>http://deanships.su.edu.sa/AR/listOfTheStudy/Pages/reg.aspx#:~:text=%D9%87)%20%D8%AA%D8%A7%D8%A8%D8%B9%20%D8%A7%D9%84%D9%82%D8%A7%D8%B9%D8%AF%D8%A9%20%D8%A7%D9%84%D8%AA%D9%86%D9%81%D9%8A%D8%B0%D9%8A%D8%A9%20%D9%84%D8%B4%D8%B1%D9%88%D8%B7,30%20%25%20%D9%84%D8%AF%D8%B1%D8%AC%D8%A9%20%D8%A7%D9%84%D8%A7%D8%AE%D8%AA%D8%A8%D8%A7%D8%B1%20%D8%A7%D9%84%D8%AA%D8%AD%D8%B5%D9%8A%D9%84%D9%8A%20)%20.</t>
+  </si>
+  <si>
+    <t>https://www.su.edu.sa/ar</t>
+  </si>
+  <si>
+    <t>https://dar.psau.edu.sa/ar/page/1-317</t>
+  </si>
+  <si>
+    <t>https://dar.psau.edu.sa/ar</t>
   </si>
 </sst>
 </file>
@@ -137,15 +182,39 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -153,14 +222,41 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -476,175 +572,304 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B29"/>
+  <dimension ref="A1:D29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="28.5" customWidth="1"/>
+    <col min="1" max="1" width="27.6640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="6" style="2" customWidth="1"/>
+    <col min="3" max="3" width="66.6640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="41.1640625" style="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+      <c r="B1" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="5"/>
+      <c r="D1" s="8"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+      <c r="B2" s="4"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="8"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
+      <c r="B3" s="4"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="8"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
+      <c r="B4" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="5"/>
+      <c r="D4" s="8"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
+      <c r="B5" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" s="5"/>
+      <c r="D5" s="8"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
+      <c r="B6" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" s="5"/>
+      <c r="D6" s="8"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
+      <c r="B7" s="4"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="8"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
+      <c r="B8" s="4"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="8"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
+      <c r="B9" s="4"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="8"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
+      <c r="B10" s="4"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="8"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
+      <c r="B11" s="4"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="8"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
+      <c r="B12" s="4"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="8"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
+      <c r="B13" s="4"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="8"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="3" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
+      <c r="B14" s="4"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="8"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="s">
+      <c r="B15" s="4"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="8"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="3" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
+      <c r="B16" s="4"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="8"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" s="1" t="s">
+      <c r="B17" s="4"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="8"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="3" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" s="1" t="s">
+      <c r="B18" s="4"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="8"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" s="1" t="s">
+      <c r="B19" s="4"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="8"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B20" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" s="1" t="s">
+      <c r="B20" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C20" s="5"/>
+      <c r="D20" s="8"/>
+    </row>
+    <row r="21" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="11" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22" s="1" t="s">
+      <c r="B21" s="12"/>
+      <c r="C21" s="12"/>
+      <c r="D21" s="12"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23" s="1" t="s">
+      <c r="B22" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" s="3" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24" s="1" t="s">
+      <c r="B23" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" s="3" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A25" s="1" t="s">
+      <c r="B24" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" s="3" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A26" s="1" t="s">
+      <c r="B25" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" s="3" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A27" s="1" t="s">
+      <c r="B26" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" s="3" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A28" s="1" t="s">
+      <c r="B27" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D27" s="9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="11" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A29" s="1" t="s">
+      <c r="B28" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="C28" s="12"/>
+      <c r="D28" s="12"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" s="3" t="s">
         <v>28</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -678,6 +903,20 @@
     <hyperlink ref="A27" r:id="rId27" display="https://www.moe.gov.sa/ar/HighEducation/Government-Universities/Pages/bisha.aspx"/>
     <hyperlink ref="A28" r:id="rId28" display="https://www.moe.gov.sa/ar/HighEducation/Government-Universities/ListOfUniversities/Pages/KingAbdullahUniversity.aspx"/>
     <hyperlink ref="A29" r:id="rId29" display="https://www.moe.gov.sa/ar/HighEducation/Government-Universities/Pages/hafr.aspx"/>
+    <hyperlink ref="C29" r:id="rId30"/>
+    <hyperlink ref="D27" r:id="rId31"/>
+    <hyperlink ref="C27" r:id="rId32"/>
+    <hyperlink ref="D29" r:id="rId33"/>
+    <hyperlink ref="C26" r:id="rId34" location=":~:text=%D9%85%D8%B9%D8%A7%D9%8A%D9%8A%D9%80%D8%B1%20%D8%A7%D9%84%D9%82%D8%A8%D9%80%D9%88%D9%84%20%D8%A8%D8%AC%D8%A7%D9%85%D8%B9%D8%A9%20%D8%AC%D8%AF%D8%A9%20%3A&amp;text=%D8%A7%D9%84%D8%AF%D8%B1%D8%AC%D8%A9%20%D8%A7%D9%84%D9%85%D9%88%D8%B2%D9%88%D9%86%D8%A9%20%D9%84%D9%84%D8%B3%D9%86%D8%A9%20%D8%A7%D9%84%D8%AA%D8%AD%D8%B6%D9%8A%D8%B1%D9%8A%D8%A9%20%D8%A7%D9%84%D9%85%D8%B3%D8%A7%D8%B1,%D8%AF%D8%B1%D8%AC%D8%A9%20%D8%A7%D9%84%D8%AA%D8%AD%D8%B5%D9%8A%D9%84%D9%8A%20%C3%97%2020%25).&amp;text=%D8%A7%D9%84%D8%AF%D8%B1%D8%AC%D8%A9%20%D8%A7%D9%84%D9%85%D9%88%D8%B2%D9%88%D9%86%D8%A9%20%D9%84%D9%84%D8%B3%D9%86%D8%A9%20%D8%A7%D9%84%D8%AA%D8%AD%D8%B6%D9%8A%D8%B1%D9%8A%D8%A9%20%D8%A7%D9%84%D9%85%D8%B3%D8%A7%D8%B1%20%D8%A7%D9%84%D8%A3%D8%AF%D8%A8%D9%8A%20(%D8%B7%D9%84%D8%A7%D8%A8)%20%3D%20(%20%D9%86%D8%B3%D8%A8%D8%A9,%D8%AF%D8%B1%D8%AC%D8%A9%20%D8%A7%D9%84%D9%82%D8%AF%D8%B1%D8%A7%D8%AA%20%C3%97%2040%25%20)." display="https://www.uj.edu.sa/Pages-Acceptance.aspx - :~:text=%D9%85%D8%B9%D8%A7%D9%8A%D9%8A%D9%80%D8%B1%20%D8%A7%D9%84%D9%82%D8%A8%D9%80%D9%88%D9%84%20%D8%A8%D8%AC%D8%A7%D9%85%D8%B9%D8%A9%20%D8%AC%D8%AF%D8%A9%20%3A&amp;text=%D8%A7%D9%84%D8%AF%D8%B1%D8%AC%D8%A9%20%D8%A7%D9%84%D9%85%D9%88%D8%B2%D9%88%D9%86%D8%A9%20%D9%84%D9%84%D8%B3%D9%86%D8%A9%20%D8%A7%D9%84%D8%AA%D8%AD%D8%B6%D9%8A%D8%B1%D9%8A%D8%A9%20%D8%A7%D9%84%D9%85%D8%B3%D8%A7%D8%B1,%D8%AF%D8%B1%D8%AC%D8%A9%20%D8%A7%D9%84%D8%AA%D8%AD%D8%B5%D9%8A%D9%84%D9%8A%20%C3%97%2020%25).&amp;text=%D8%A7%D9%84%D8%AF%D8%B1%D8%AC%D8%A9%20%D8%A7%D9%84%D9%85%D9%88%D8%B2%D9%88%D9%86%D8%A9%20%D9%84%D9%84%D8%B3%D9%86%D8%A9%20%D8%A7%D9%84%D8%AA%D8%AD%D8%B6%D9%8A%D8%B1%D9%8A%D8%A9%20%D8%A7%D9%84%D9%85%D8%B3%D8%A7%D8%B1%20%D8%A7%D9%84%D8%A3%D8%AF%D8%A8%D9%8A%20(%D8%B7%D9%84%D8%A7%D8%A8)%20%3D%20(%20%D9%86%D8%B3%D8%A8%D8%A9,%D8%AF%D8%B1%D8%AC%D8%A9%20%D8%A7%D9%84%D9%82%D8%AF%D8%B1%D8%A7%D8%AA%20%C3%97%2040%25%20)."/>
+    <hyperlink ref="D26" r:id="rId35"/>
+    <hyperlink ref="C25" r:id="rId36"/>
+    <hyperlink ref="D25" r:id="rId37" display="https://www.seu.edu.sa/ar/"/>
+    <hyperlink ref="C24" r:id="rId38" display="http://m.mu.edu.sa/ar/%D8%A7%D9%84%D8%A7%D8%AF%D8%A7%D8%B1%D8%A7%D8%AA/%D8%B9%D9%85%D8%A7%D8%AF%D8%A9-%D8%A7%D9%84%D9%82%D8%A8%D9%88%D9%84-%D9%88%D8%A7%D9%84%D8%AA%D8%B3%D8%AC%D9%8A%D9%84/%D9%85%D8%B9%D8%A7%D9%8A%D9%8A%D8%B1-%D8%A7%D9%84%D9%82%D8%A8%D9%88%D9%84-%D8%A8%D8%AC%D8%A7%D9%85%D8%B9%D8%A9-%D8%A7%D9%84%D9%85%D8%AC%D9%85%D8%B9%D8%A9"/>
+    <hyperlink ref="D24" r:id="rId39"/>
+    <hyperlink ref="C23" r:id="rId40" location=":~:text=%D9%87)%20%D8%AA%D8%A7%D8%A8%D8%B9%20%D8%A7%D9%84%D9%82%D8%A7%D8%B9%D8%AF%D8%A9%20%D8%A7%D9%84%D8%AA%D9%86%D9%81%D9%8A%D8%B0%D9%8A%D8%A9%20%D9%84%D8%B4%D8%B1%D9%88%D8%B7,30%20%25%20%D9%84%D8%AF%D8%B1%D8%AC%D8%A9%20%D8%A7%D9%84%D8%A7%D8%AE%D8%AA%D8%A8%D8%A7%D8%B1%20%D8%A7%D9%84%D8%AA%D8%AD%D8%B5%D9%8A%D9%84%D9%8A%20)%20." display="http://deanships.su.edu.sa/AR/listOfTheStudy/Pages/reg.aspx - :~:text=%D9%87)%20%D8%AA%D8%A7%D8%A8%D8%B9%20%D8%A7%D9%84%D9%82%D8%A7%D8%B9%D8%AF%D8%A9%20%D8%A7%D9%84%D8%AA%D9%86%D9%81%D9%8A%D8%B0%D9%8A%D8%A9%20%D9%84%D8%B4%D8%B1%D9%88%D8%B7,30%20%25%20%D9%84%D8%AF%D8%B1%D8%AC%D8%A9%20%D8%A7%D9%84%D8%A7%D8%AE%D8%AA%D8%A8%D8%A7%D8%B1%20%D8%A7%D9%84%D8%AA%D8%AD%D8%B5%D9%8A%D9%84%D9%8A%20)%20."/>
+    <hyperlink ref="D23" r:id="rId41"/>
+    <hyperlink ref="C22" r:id="rId42"/>
+    <hyperlink ref="D22" r:id="rId43"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>